<commit_message>
Anunt despre restantele online
</commit_message>
<xml_diff>
--- a/LC-lab-info1s1.xlsx
+++ b/LC-lab-info1s1.xlsx
@@ -5,18 +5,18 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://storage.rcs-rds.ro/dav/Digi Cloud/Ovidius_Studenti/INFO1s1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\axa\Documents\Reps\andrei-rusu-ovidius.github.io\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AA0D193-843F-46D7-93D7-65AA969421BC}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F4C4445-9996-409C-859A-2323BEA708C6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="730" yWindow="1320" windowWidth="9680" windowHeight="9000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table 1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Table 1'!$A$15:$L$15</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Table 1'!$A$15:$M$15</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="133">
   <si>
     <r>
       <rPr>
@@ -706,6 +706,45 @@
   </si>
   <si>
     <t>Legendă: x - încărcat pe server storage, y - îl am pe email</t>
+  </si>
+  <si>
+    <t>alexandru.chiriacescu@365.univ-ovidius.ro</t>
+  </si>
+  <si>
+    <t>george.enciu@365.univ-ovidius.ro</t>
+  </si>
+  <si>
+    <t>dearboom6@gmail.com</t>
+  </si>
+  <si>
+    <t>andrei.lepadatu@365.univ-ovidius.ro</t>
+  </si>
+  <si>
+    <t>vlad.ispir.2000@gmail.com</t>
+  </si>
+  <si>
+    <t>alin.chetran@365.univ-ovidius.ro</t>
+  </si>
+  <si>
+    <t>vlad.antonaru@365.univ-ovidius.ro</t>
+  </si>
+  <si>
+    <t>Sandu Vasile Bogdan</t>
+  </si>
+  <si>
+    <t>bogdan.sandu@365.univ-ovidius.ro</t>
+  </si>
+  <si>
+    <t>claudiudragan07@yahoo.com</t>
+  </si>
+  <si>
+    <t>radu.badeanu@365.univ-ovidius.ro</t>
+  </si>
+  <si>
+    <t>flore.evg@gmail.com</t>
+  </si>
+  <si>
+    <t>romaniahp@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -847,7 +886,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -910,6 +949,30 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="1" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1249,92 +1312,117 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L90"/>
+  <dimension ref="A1:M93"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="15" topLeftCell="E16" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="15" topLeftCell="J45" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A9" sqref="A9"/>
       <selection pane="topRight" activeCell="E9" sqref="E9"/>
       <selection pane="bottomLeft" activeCell="A16" sqref="A16"/>
-      <selection pane="bottomRight" activeCell="K90" sqref="A1:K90"/>
+      <selection pane="bottomRight" activeCell="J52" sqref="J52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="5.796875" customWidth="1"/>
-    <col min="2" max="2" width="58.19921875" customWidth="1"/>
-    <col min="3" max="3" width="10.69921875" customWidth="1"/>
-    <col min="4" max="4" width="6.796875" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="11" width="6.19921875" customWidth="1"/>
-    <col min="12" max="12" width="32.19921875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.5" customWidth="1"/>
+    <col min="3" max="3" width="10.69921875" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="4.5" customWidth="1"/>
+    <col min="5" max="5" width="6" style="4" customWidth="1"/>
+    <col min="6" max="10" width="6" customWidth="1"/>
+    <col min="11" max="11" width="6" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="6" customWidth="1"/>
+    <col min="13" max="13" width="32.19921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="22.5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="13" spans="1:13" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="14" spans="1:13" ht="22.5" x14ac:dyDescent="0.3">
       <c r="A14" s="10" t="s">
         <v>90</v>
       </c>
       <c r="B14" s="10"/>
-      <c r="E14">
-        <f>COUNTA(E16:E88)</f>
-        <v>19</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" s="5" customFormat="1" ht="39" x14ac:dyDescent="0.3">
+      <c r="F14">
+        <f>COUNTA(F16:F88)</f>
+        <v>37</v>
+      </c>
+      <c r="G14">
+        <f t="shared" ref="G14:K14" si="0">COUNTA(G16:G88)</f>
+        <v>28</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="J14">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="K14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" s="5" customFormat="1" ht="39" x14ac:dyDescent="0.3">
       <c r="A15" s="6" t="s">
         <v>39</v>
       </c>
@@ -1344,35 +1432,36 @@
       <c r="C15" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="D15" s="14" t="s">
+      <c r="D15" s="28"/>
+      <c r="E15" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="E15" s="15" t="s">
+      <c r="F15" s="15" t="s">
         <v>92</v>
       </c>
-      <c r="F15" s="15" t="s">
+      <c r="G15" s="15" t="s">
         <v>93</v>
       </c>
-      <c r="G15" s="15" t="s">
+      <c r="H15" s="15" t="s">
         <v>94</v>
       </c>
-      <c r="H15" s="15" t="s">
+      <c r="I15" s="15" t="s">
         <v>95</v>
       </c>
-      <c r="I15" s="15" t="s">
+      <c r="J15" s="15" t="s">
         <v>96</v>
       </c>
-      <c r="J15" s="15" t="s">
+      <c r="K15" s="15" t="s">
         <v>97</v>
       </c>
-      <c r="K15" s="15" t="s">
+      <c r="L15" s="15" t="s">
         <v>118</v>
       </c>
-      <c r="L15" s="18" t="s">
+      <c r="M15" s="18" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="15.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" ht="15.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="8">
         <v>1</v>
       </c>
@@ -1382,22 +1471,26 @@
       <c r="C16" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="D16" s="16">
+      <c r="D16" s="27" t="str">
+        <f t="shared" ref="D16:D23" si="1">IF(COUNTA(F16:K16)=0,"",COUNTA(F16:K16))</f>
+        <v/>
+      </c>
+      <c r="E16" s="16">
         <v>1</v>
       </c>
-      <c r="E16" s="16"/>
       <c r="F16" s="16"/>
       <c r="G16" s="16"/>
       <c r="H16" s="16"/>
       <c r="I16" s="16"/>
       <c r="J16" s="16"/>
-      <c r="K16" s="16" t="str">
-        <f>IF(L16&lt;&gt;"","Da","Nu")</f>
-        <v>Nu</v>
-      </c>
-      <c r="L16" s="19"/>
-    </row>
-    <row r="17" spans="1:12" ht="15.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="K16" s="16"/>
+      <c r="L16" s="16" t="str">
+        <f>IF(M16&lt;&gt;"","Da","Nu")</f>
+        <v>Nu</v>
+      </c>
+      <c r="M16" s="19"/>
+    </row>
+    <row r="17" spans="1:13" ht="15.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="8">
         <v>2</v>
       </c>
@@ -1407,22 +1500,28 @@
       <c r="C17" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="D17" s="16">
+      <c r="D17" s="27">
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="E17" s="16"/>
+      <c r="E17" s="16">
+        <v>1</v>
+      </c>
       <c r="F17" s="16"/>
       <c r="G17" s="16"/>
-      <c r="H17" s="16"/>
+      <c r="H17" s="17" t="s">
+        <v>100</v>
+      </c>
       <c r="I17" s="16"/>
       <c r="J17" s="16"/>
-      <c r="K17" s="16" t="str">
-        <f t="shared" ref="K17:K80" si="0">IF(L17&lt;&gt;"","Da","Nu")</f>
-        <v>Nu</v>
-      </c>
-      <c r="L17" s="19"/>
-    </row>
-    <row r="18" spans="1:12" ht="15.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="K17" s="16"/>
+      <c r="L17" s="16" t="str">
+        <f>IF(M17&lt;&gt;"","Da","Nu")</f>
+        <v>Nu</v>
+      </c>
+      <c r="M17" s="19"/>
+    </row>
+    <row r="18" spans="1:13" ht="15.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="8">
         <v>3</v>
       </c>
@@ -1432,22 +1531,26 @@
       <c r="C18" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="D18" s="16">
+      <c r="D18" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="E18" s="16">
         <v>1</v>
       </c>
-      <c r="E18" s="16"/>
       <c r="F18" s="16"/>
       <c r="G18" s="16"/>
       <c r="H18" s="16"/>
       <c r="I18" s="16"/>
       <c r="J18" s="16"/>
-      <c r="K18" s="16" t="str">
-        <f t="shared" si="0"/>
-        <v>Nu</v>
-      </c>
-      <c r="L18" s="19"/>
-    </row>
-    <row r="19" spans="1:12" ht="15.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="K18" s="16"/>
+      <c r="L18" s="16" t="str">
+        <f>IF(M18&lt;&gt;"","Da","Nu")</f>
+        <v>Nu</v>
+      </c>
+      <c r="M18" s="19"/>
+    </row>
+    <row r="19" spans="1:13" ht="15.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="8">
         <v>4</v>
       </c>
@@ -1457,12 +1560,13 @@
       <c r="C19" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="D19" s="16">
+      <c r="D19" s="27">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="E19" s="16">
         <v>1</v>
       </c>
-      <c r="E19" s="17" t="s">
-        <v>100</v>
-      </c>
       <c r="F19" s="17" t="s">
         <v>100</v>
       </c>
@@ -1475,72 +1579,83 @@
       <c r="I19" s="17" t="s">
         <v>100</v>
       </c>
-      <c r="J19" s="16"/>
-      <c r="K19" s="16" t="str">
-        <f t="shared" si="0"/>
+      <c r="J19" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="K19" s="16"/>
+      <c r="L19" s="16" t="str">
+        <f>IF(M19&lt;&gt;"","Da","Nu")</f>
         <v>Da</v>
       </c>
-      <c r="L19" s="19" t="s">
+      <c r="M19" s="19" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="20" spans="1:12" ht="15.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:13" ht="15.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="8">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="D20" s="16">
+        <v>41</v>
+      </c>
+      <c r="D20" s="27">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="E20" s="16">
         <v>1</v>
       </c>
-      <c r="E20" s="16"/>
-      <c r="F20" s="16"/>
-      <c r="G20" s="16"/>
+      <c r="F20" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="G20" s="17" t="s">
+        <v>100</v>
+      </c>
       <c r="H20" s="16"/>
       <c r="I20" s="16"/>
       <c r="J20" s="16"/>
-      <c r="K20" s="16" t="str">
-        <f t="shared" si="0"/>
-        <v>Nu</v>
-      </c>
-      <c r="L20" s="19"/>
-    </row>
-    <row r="21" spans="1:12" ht="15.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="K20" s="16"/>
+      <c r="L20" s="16" t="str">
+        <f>IF(M20&lt;&gt;"","Da","Nu")</f>
+        <v>Da</v>
+      </c>
+      <c r="M20" s="19" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" ht="15.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="8">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="D21" s="16">
+        <v>43</v>
+      </c>
+      <c r="D21" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="E21" s="16">
         <v>1</v>
       </c>
-      <c r="E21" s="17" t="s">
-        <v>100</v>
-      </c>
-      <c r="F21" s="17" t="s">
-        <v>100</v>
-      </c>
+      <c r="F21" s="16"/>
       <c r="G21" s="16"/>
       <c r="H21" s="16"/>
       <c r="I21" s="16"/>
       <c r="J21" s="16"/>
-      <c r="K21" s="16" t="str">
-        <f t="shared" si="0"/>
-        <v>Da</v>
-      </c>
-      <c r="L21" s="19" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" ht="15.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="K21" s="16"/>
+      <c r="L21" s="16" t="str">
+        <f>IF(M21&lt;&gt;"","Da","Nu")</f>
+        <v>Nu</v>
+      </c>
+      <c r="M21" s="19"/>
+    </row>
+    <row r="22" spans="1:13" ht="15.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="8">
         <v>7</v>
       </c>
@@ -1550,22 +1665,30 @@
       <c r="C22" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="D22" s="16">
+      <c r="D22" s="27">
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="E22" s="16"/>
-      <c r="F22" s="16"/>
+      <c r="E22" s="16">
+        <v>1</v>
+      </c>
+      <c r="F22" s="17" t="s">
+        <v>100</v>
+      </c>
       <c r="G22" s="16"/>
       <c r="H22" s="16"/>
       <c r="I22" s="16"/>
       <c r="J22" s="16"/>
-      <c r="K22" s="16" t="str">
-        <f t="shared" si="0"/>
-        <v>Nu</v>
-      </c>
-      <c r="L22" s="19"/>
-    </row>
-    <row r="23" spans="1:12" ht="15.65" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="K22" s="16"/>
+      <c r="L22" s="16" t="str">
+        <f>IF(M22&lt;&gt;"","Da","Nu")</f>
+        <v>Da</v>
+      </c>
+      <c r="M22" s="19" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" ht="15.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="8">
         <v>8</v>
       </c>
@@ -1575,22 +1698,30 @@
       <c r="C23" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="D23" s="16">
+      <c r="D23" s="27">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="E23" s="16">
         <v>1</v>
       </c>
-      <c r="E23" s="16"/>
-      <c r="F23" s="16"/>
-      <c r="G23" s="16"/>
+      <c r="F23" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="G23" s="17" t="s">
+        <v>100</v>
+      </c>
       <c r="H23" s="16"/>
       <c r="I23" s="16"/>
       <c r="J23" s="16"/>
-      <c r="K23" s="16" t="str">
-        <f t="shared" si="0"/>
-        <v>Nu</v>
-      </c>
-      <c r="L23" s="19"/>
-    </row>
-    <row r="24" spans="1:12" ht="15.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="K23" s="16"/>
+      <c r="L23" s="16" t="str">
+        <f>IF(M23&lt;&gt;"","Da","Nu")</f>
+        <v>Nu</v>
+      </c>
+      <c r="M23" s="19"/>
+    </row>
+    <row r="24" spans="1:13" ht="15.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="8">
         <v>9</v>
       </c>
@@ -1600,12 +1731,13 @@
       <c r="C24" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="D24" s="16">
+      <c r="D24" s="27">
+        <f>IF(COUNTA(F24:K24)=0,"",COUNTA(F24:K24))</f>
+        <v>5</v>
+      </c>
+      <c r="E24" s="16">
         <v>1</v>
       </c>
-      <c r="E24" s="17" t="s">
-        <v>100</v>
-      </c>
       <c r="F24" s="17" t="s">
         <v>100</v>
       </c>
@@ -1618,16 +1750,19 @@
       <c r="I24" s="17" t="s">
         <v>100</v>
       </c>
-      <c r="J24" s="16"/>
-      <c r="K24" s="16" t="str">
-        <f t="shared" si="0"/>
+      <c r="J24" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="K24" s="16"/>
+      <c r="L24" s="16" t="str">
+        <f>IF(M24&lt;&gt;"","Da","Nu")</f>
         <v>Da</v>
       </c>
-      <c r="L24" s="19" t="s">
+      <c r="M24" s="19" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="25" spans="1:12" ht="15.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:13" ht="15.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="8">
         <v>10</v>
       </c>
@@ -1637,72 +1772,94 @@
       <c r="C25" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="D25" s="16">
+      <c r="D25" s="27" t="str">
+        <f t="shared" ref="D25:D88" si="2">IF(COUNTA(F25:K25)=0,"",COUNTA(F25:K25))</f>
+        <v/>
+      </c>
+      <c r="E25" s="16">
         <v>1</v>
       </c>
-      <c r="E25" s="16"/>
       <c r="F25" s="16"/>
       <c r="G25" s="16"/>
       <c r="H25" s="16"/>
       <c r="I25" s="16"/>
       <c r="J25" s="16"/>
-      <c r="K25" s="16" t="str">
-        <f t="shared" si="0"/>
-        <v>Nu</v>
-      </c>
-      <c r="L25" s="19"/>
-    </row>
-    <row r="26" spans="1:12" ht="15.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="K25" s="16"/>
+      <c r="L25" s="16" t="str">
+        <f>IF(M25&lt;&gt;"","Da","Nu")</f>
+        <v>Nu</v>
+      </c>
+      <c r="M25" s="19"/>
+    </row>
+    <row r="26" spans="1:13" ht="15.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="8">
+        <v>12</v>
+      </c>
+      <c r="B26" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="C26" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="D26" s="27">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="E26" s="16">
+        <v>1</v>
+      </c>
+      <c r="F26" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="G26" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="H26" s="16"/>
+      <c r="I26" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="J26" s="16"/>
+      <c r="K26" s="16"/>
+      <c r="L26" s="16" t="str">
+        <f>IF(M26&lt;&gt;"","Da","Nu")</f>
+        <v>Da</v>
+      </c>
+      <c r="M26" s="19" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" ht="15.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="8">
         <v>11</v>
       </c>
-      <c r="B26" s="9" t="s">
+      <c r="B27" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="C26" s="12" t="s">
+      <c r="C27" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="D26" s="16">
+      <c r="D27" s="27">
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="E26" s="16"/>
-      <c r="F26" s="16"/>
-      <c r="G26" s="16"/>
-      <c r="H26" s="16"/>
-      <c r="I26" s="16"/>
-      <c r="J26" s="16"/>
-      <c r="K26" s="16" t="str">
-        <f t="shared" si="0"/>
-        <v>Nu</v>
-      </c>
-      <c r="L26" s="19"/>
-    </row>
-    <row r="27" spans="1:12" ht="15.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="8">
-        <v>12</v>
-      </c>
-      <c r="B27" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="C27" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="D27" s="16">
+      <c r="E27" s="16">
         <v>1</v>
       </c>
-      <c r="E27" s="16"/>
-      <c r="F27" s="16"/>
+      <c r="F27" s="17" t="s">
+        <v>100</v>
+      </c>
       <c r="G27" s="16"/>
       <c r="H27" s="16"/>
       <c r="I27" s="16"/>
       <c r="J27" s="16"/>
-      <c r="K27" s="16" t="str">
-        <f t="shared" si="0"/>
-        <v>Nu</v>
-      </c>
-      <c r="L27" s="19"/>
-    </row>
-    <row r="28" spans="1:12" ht="15.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="K27" s="16"/>
+      <c r="L27" s="16" t="str">
+        <f>IF(M27&lt;&gt;"","Da","Nu")</f>
+        <v>Nu</v>
+      </c>
+      <c r="M27" s="19"/>
+    </row>
+    <row r="28" spans="1:13" ht="15.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="8">
         <v>13</v>
       </c>
@@ -1712,22 +1869,26 @@
       <c r="C28" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="D28" s="16">
+      <c r="D28" s="27" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="E28" s="16">
         <v>1</v>
       </c>
-      <c r="E28" s="16"/>
       <c r="F28" s="16"/>
       <c r="G28" s="16"/>
       <c r="H28" s="16"/>
       <c r="I28" s="16"/>
       <c r="J28" s="16"/>
-      <c r="K28" s="16" t="str">
-        <f t="shared" si="0"/>
-        <v>Nu</v>
-      </c>
-      <c r="L28" s="19"/>
-    </row>
-    <row r="29" spans="1:12" ht="15.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="K28" s="16"/>
+      <c r="L28" s="16" t="str">
+        <f>IF(M28&lt;&gt;"","Da","Nu")</f>
+        <v>Nu</v>
+      </c>
+      <c r="M28" s="19"/>
+    </row>
+    <row r="29" spans="1:13" ht="15.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="8">
         <v>14</v>
       </c>
@@ -1737,22 +1898,26 @@
       <c r="C29" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="D29" s="16">
+      <c r="D29" s="27" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="E29" s="16">
         <v>1</v>
       </c>
-      <c r="E29" s="16"/>
       <c r="F29" s="16"/>
       <c r="G29" s="16"/>
       <c r="H29" s="16"/>
       <c r="I29" s="16"/>
       <c r="J29" s="16"/>
-      <c r="K29" s="16" t="str">
-        <f t="shared" si="0"/>
-        <v>Nu</v>
-      </c>
-      <c r="L29" s="19"/>
-    </row>
-    <row r="30" spans="1:12" ht="15.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="K29" s="16"/>
+      <c r="L29" s="16" t="str">
+        <f>IF(M29&lt;&gt;"","Da","Nu")</f>
+        <v>Nu</v>
+      </c>
+      <c r="M29" s="19"/>
+    </row>
+    <row r="30" spans="1:13" ht="15.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="8">
         <v>15</v>
       </c>
@@ -1762,22 +1927,26 @@
       <c r="C30" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="D30" s="16">
+      <c r="D30" s="27" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="E30" s="16">
         <v>1</v>
       </c>
-      <c r="E30" s="16"/>
       <c r="F30" s="16"/>
       <c r="G30" s="16"/>
       <c r="H30" s="16"/>
       <c r="I30" s="16"/>
       <c r="J30" s="16"/>
-      <c r="K30" s="16" t="str">
-        <f t="shared" si="0"/>
-        <v>Nu</v>
-      </c>
-      <c r="L30" s="19"/>
-    </row>
-    <row r="31" spans="1:12" ht="15.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="K30" s="16"/>
+      <c r="L30" s="16" t="str">
+        <f>IF(M30&lt;&gt;"","Da","Nu")</f>
+        <v>Nu</v>
+      </c>
+      <c r="M30" s="19"/>
+    </row>
+    <row r="31" spans="1:13" ht="15.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="8">
         <v>16</v>
       </c>
@@ -1787,22 +1956,26 @@
       <c r="C31" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="D31" s="16">
+      <c r="D31" s="27" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="E31" s="16">
         <v>1</v>
       </c>
-      <c r="E31" s="16"/>
       <c r="F31" s="16"/>
       <c r="G31" s="16"/>
       <c r="H31" s="16"/>
       <c r="I31" s="16"/>
       <c r="J31" s="16"/>
-      <c r="K31" s="16" t="str">
-        <f t="shared" si="0"/>
-        <v>Nu</v>
-      </c>
-      <c r="L31" s="19"/>
-    </row>
-    <row r="32" spans="1:12" ht="15.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="K31" s="16"/>
+      <c r="L31" s="16" t="str">
+        <f>IF(M31&lt;&gt;"","Da","Nu")</f>
+        <v>Nu</v>
+      </c>
+      <c r="M31" s="19"/>
+    </row>
+    <row r="32" spans="1:13" ht="15.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="8">
         <v>17</v>
       </c>
@@ -1812,22 +1985,30 @@
       <c r="C32" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="D32" s="16">
+      <c r="D32" s="27">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="E32" s="16">
         <v>1</v>
       </c>
-      <c r="E32" s="16"/>
-      <c r="F32" s="16"/>
-      <c r="G32" s="16"/>
+      <c r="F32" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="G32" s="17" t="s">
+        <v>100</v>
+      </c>
       <c r="H32" s="16"/>
       <c r="I32" s="16"/>
       <c r="J32" s="16"/>
-      <c r="K32" s="16" t="str">
-        <f t="shared" si="0"/>
-        <v>Nu</v>
-      </c>
-      <c r="L32" s="19"/>
-    </row>
-    <row r="33" spans="1:12" ht="15.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="K32" s="16"/>
+      <c r="L32" s="16" t="str">
+        <f>IF(M32&lt;&gt;"","Da","Nu")</f>
+        <v>Nu</v>
+      </c>
+      <c r="M32" s="19"/>
+    </row>
+    <row r="33" spans="1:13" ht="15.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="8">
         <v>18</v>
       </c>
@@ -1837,28 +2018,32 @@
       <c r="C33" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="D33" s="16">
+      <c r="D33" s="27">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="E33" s="16">
         <v>1</v>
       </c>
-      <c r="E33" s="17" t="s">
-        <v>100</v>
-      </c>
       <c r="F33" s="17" t="s">
         <v>100</v>
       </c>
-      <c r="G33" s="16"/>
+      <c r="G33" s="17" t="s">
+        <v>100</v>
+      </c>
       <c r="H33" s="16"/>
       <c r="I33" s="16"/>
       <c r="J33" s="16"/>
-      <c r="K33" s="16" t="str">
-        <f t="shared" si="0"/>
+      <c r="K33" s="16"/>
+      <c r="L33" s="16" t="str">
+        <f>IF(M33&lt;&gt;"","Da","Nu")</f>
         <v>Da</v>
       </c>
-      <c r="L33" s="19" t="s">
+      <c r="M33" s="19" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="34" spans="1:12" ht="15.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:13" ht="15.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="8">
         <v>19</v>
       </c>
@@ -1868,12 +2053,13 @@
       <c r="C34" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="D34" s="16">
+      <c r="D34" s="27">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="E34" s="16">
         <v>1</v>
       </c>
-      <c r="E34" s="17" t="s">
-        <v>100</v>
-      </c>
       <c r="F34" s="17" t="s">
         <v>100</v>
       </c>
@@ -1883,17 +2069,22 @@
       <c r="H34" s="17" t="s">
         <v>100</v>
       </c>
-      <c r="I34" s="16"/>
-      <c r="J34" s="16"/>
-      <c r="K34" s="16" t="str">
-        <f t="shared" si="0"/>
+      <c r="I34" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="J34" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="K34" s="16"/>
+      <c r="L34" s="16" t="str">
+        <f>IF(M34&lt;&gt;"","Da","Nu")</f>
         <v>Da</v>
       </c>
-      <c r="L34" s="20" t="s">
+      <c r="M34" s="20" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="35" spans="1:12" ht="15.65" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:13" ht="15.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="8">
         <v>20</v>
       </c>
@@ -1903,72 +2094,84 @@
       <c r="C35" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="D35" s="16">
+      <c r="D35" s="27" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="E35" s="16">
         <v>1</v>
       </c>
-      <c r="E35" s="16"/>
       <c r="F35" s="16"/>
       <c r="G35" s="16"/>
       <c r="H35" s="16"/>
       <c r="I35" s="16"/>
       <c r="J35" s="16"/>
-      <c r="K35" s="16" t="str">
-        <f t="shared" si="0"/>
-        <v>Nu</v>
-      </c>
-      <c r="L35" s="19"/>
-    </row>
-    <row r="36" spans="1:12" ht="15.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="K35" s="16"/>
+      <c r="L35" s="16" t="str">
+        <f>IF(M35&lt;&gt;"","Da","Nu")</f>
+        <v>Nu</v>
+      </c>
+      <c r="M35" s="19"/>
+    </row>
+    <row r="36" spans="1:13" ht="15.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="8">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B36" s="9" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C36" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="D36" s="16">
+      <c r="D36" s="27" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="E36" s="16">
         <v>1</v>
       </c>
-      <c r="E36" s="16"/>
       <c r="F36" s="16"/>
       <c r="G36" s="16"/>
       <c r="H36" s="16"/>
       <c r="I36" s="16"/>
       <c r="J36" s="16"/>
-      <c r="K36" s="16" t="str">
-        <f t="shared" si="0"/>
-        <v>Nu</v>
-      </c>
-      <c r="L36" s="19"/>
-    </row>
-    <row r="37" spans="1:12" ht="15.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="K36" s="16"/>
+      <c r="L36" s="16" t="str">
+        <f>IF(M36&lt;&gt;"","Da","Nu")</f>
+        <v>Nu</v>
+      </c>
+      <c r="M36" s="19"/>
+    </row>
+    <row r="37" spans="1:13" ht="15.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="8">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B37" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C37" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="D37" s="16">
+      <c r="D37" s="27" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="E37" s="16">
         <v>1</v>
       </c>
-      <c r="E37" s="16"/>
       <c r="F37" s="16"/>
       <c r="G37" s="16"/>
       <c r="H37" s="16"/>
       <c r="I37" s="16"/>
       <c r="J37" s="16"/>
-      <c r="K37" s="16" t="str">
-        <f t="shared" si="0"/>
-        <v>Nu</v>
-      </c>
-      <c r="L37" s="19"/>
-    </row>
-    <row r="38" spans="1:12" ht="15.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="K37" s="16"/>
+      <c r="L37" s="16" t="str">
+        <f>IF(M37&lt;&gt;"","Da","Nu")</f>
+        <v>Nu</v>
+      </c>
+      <c r="M37" s="19"/>
+    </row>
+    <row r="38" spans="1:13" ht="15.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="8">
         <v>23</v>
       </c>
@@ -1978,22 +2181,26 @@
       <c r="C38" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="D38" s="16">
+      <c r="D38" s="27" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="E38" s="16">
         <v>1</v>
       </c>
-      <c r="E38" s="16"/>
       <c r="F38" s="16"/>
       <c r="G38" s="16"/>
       <c r="H38" s="16"/>
       <c r="I38" s="16"/>
       <c r="J38" s="16"/>
-      <c r="K38" s="16" t="str">
-        <f t="shared" si="0"/>
-        <v>Nu</v>
-      </c>
-      <c r="L38" s="19"/>
-    </row>
-    <row r="39" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="K38" s="16"/>
+      <c r="L38" s="16" t="str">
+        <f>IF(M38&lt;&gt;"","Da","Nu")</f>
+        <v>Nu</v>
+      </c>
+      <c r="M38" s="19"/>
+    </row>
+    <row r="39" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="8">
         <v>24</v>
       </c>
@@ -2003,22 +2210,36 @@
       <c r="C39" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="D39" s="16">
+      <c r="D39" s="27">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="E39" s="16">
         <v>1</v>
       </c>
-      <c r="E39" s="16"/>
-      <c r="F39" s="16"/>
-      <c r="G39" s="16"/>
-      <c r="H39" s="16"/>
-      <c r="I39" s="16"/>
-      <c r="J39" s="16"/>
-      <c r="K39" s="16" t="str">
-        <f t="shared" si="0"/>
-        <v>Nu</v>
-      </c>
-      <c r="L39" s="19"/>
-    </row>
-    <row r="40" spans="1:12" ht="15.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F39" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="G39" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="H39" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="I39" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="J39" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="K39" s="16"/>
+      <c r="L39" s="16" t="str">
+        <f>IF(M39&lt;&gt;"","Da","Nu")</f>
+        <v>Nu</v>
+      </c>
+      <c r="M39" s="19"/>
+    </row>
+    <row r="40" spans="1:13" ht="15.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="8">
         <v>25</v>
       </c>
@@ -2028,130 +2249,160 @@
       <c r="C40" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="D40" s="16">
+      <c r="D40" s="27" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="E40" s="16">
         <v>2</v>
       </c>
-      <c r="E40" s="16"/>
       <c r="F40" s="16"/>
       <c r="G40" s="16"/>
       <c r="H40" s="16"/>
       <c r="I40" s="16"/>
       <c r="J40" s="16"/>
-      <c r="K40" s="16" t="str">
-        <f t="shared" si="0"/>
-        <v>Nu</v>
-      </c>
-      <c r="L40" s="19"/>
-    </row>
-    <row r="41" spans="1:12" ht="15.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="K40" s="16"/>
+      <c r="L40" s="16" t="str">
+        <f>IF(M40&lt;&gt;"","Da","Nu")</f>
+        <v>Nu</v>
+      </c>
+      <c r="M40" s="19"/>
+    </row>
+    <row r="41" spans="1:13" ht="15.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="8">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B41" s="9" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C41" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="D41" s="16">
+        <v>43</v>
+      </c>
+      <c r="D41" s="27" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="E41" s="16">
         <v>2</v>
       </c>
-      <c r="E41" s="16"/>
       <c r="F41" s="16"/>
       <c r="G41" s="16"/>
       <c r="H41" s="16"/>
       <c r="I41" s="16"/>
       <c r="J41" s="16"/>
-      <c r="K41" s="16" t="str">
-        <f t="shared" si="0"/>
-        <v>Nu</v>
-      </c>
-      <c r="L41" s="19"/>
-    </row>
-    <row r="42" spans="1:12" ht="15.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="K41" s="16"/>
+      <c r="L41" s="16" t="str">
+        <f>IF(M41&lt;&gt;"","Da","Nu")</f>
+        <v>Nu</v>
+      </c>
+      <c r="M41" s="19"/>
+    </row>
+    <row r="42" spans="1:13" ht="15.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="8">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B42" s="9" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="C42" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="D42" s="16">
+        <v>43</v>
+      </c>
+      <c r="D42" s="27" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="E42" s="16">
         <v>2</v>
       </c>
-      <c r="E42" s="17" t="s">
-        <v>100</v>
-      </c>
-      <c r="F42" s="17" t="s">
-        <v>100</v>
-      </c>
+      <c r="F42" s="16"/>
       <c r="G42" s="16"/>
-      <c r="H42" s="17" t="s">
-        <v>100</v>
-      </c>
+      <c r="H42" s="16"/>
       <c r="I42" s="16"/>
       <c r="J42" s="16"/>
-      <c r="K42" s="16" t="str">
-        <f t="shared" si="0"/>
+      <c r="K42" s="16"/>
+      <c r="L42" s="16" t="str">
+        <f>IF(M42&lt;&gt;"","Da","Nu")</f>
+        <v>Nu</v>
+      </c>
+      <c r="M42" s="19"/>
+    </row>
+    <row r="43" spans="1:13" ht="15.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="8">
+        <v>26</v>
+      </c>
+      <c r="B43" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="C43" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="D43" s="27">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="E43" s="16">
+        <v>2</v>
+      </c>
+      <c r="F43" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="G43" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="H43" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="I43" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="J43" s="16"/>
+      <c r="K43" s="16"/>
+      <c r="L43" s="16" t="str">
+        <f>IF(M43&lt;&gt;"","Da","Nu")</f>
         <v>Da</v>
       </c>
-      <c r="L42" s="19" t="s">
+      <c r="M43" s="19" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" ht="15.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="8">
+        <v>27</v>
+      </c>
+      <c r="B44" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="C44" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="D44" s="27">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="E44" s="16">
+        <v>2</v>
+      </c>
+      <c r="F44" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="G44" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="H44" s="16"/>
+      <c r="I44" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="J44" s="16"/>
+      <c r="K44" s="16"/>
+      <c r="L44" s="16" t="str">
+        <f>IF(M44&lt;&gt;"","Da","Nu")</f>
+        <v>Da</v>
+      </c>
+      <c r="M44" s="19" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="43" spans="1:12" ht="15.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="8">
-        <v>28</v>
-      </c>
-      <c r="B43" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="C43" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="D43" s="16">
-        <v>2</v>
-      </c>
-      <c r="E43" s="16"/>
-      <c r="F43" s="16"/>
-      <c r="G43" s="16"/>
-      <c r="H43" s="16"/>
-      <c r="I43" s="16"/>
-      <c r="J43" s="16"/>
-      <c r="K43" s="16" t="str">
-        <f t="shared" si="0"/>
-        <v>Nu</v>
-      </c>
-      <c r="L43" s="19"/>
-    </row>
-    <row r="44" spans="1:12" ht="15.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="8">
-        <v>29</v>
-      </c>
-      <c r="B44" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="C44" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="D44" s="16">
-        <v>2</v>
-      </c>
-      <c r="E44" s="16"/>
-      <c r="F44" s="16"/>
-      <c r="G44" s="16"/>
-      <c r="H44" s="16"/>
-      <c r="I44" s="16"/>
-      <c r="J44" s="16"/>
-      <c r="K44" s="16" t="str">
-        <f t="shared" si="0"/>
-        <v>Nu</v>
-      </c>
-      <c r="L44" s="19"/>
-    </row>
-    <row r="45" spans="1:12" ht="15.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:13" ht="15.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="8">
         <v>30</v>
       </c>
@@ -2161,22 +2412,26 @@
       <c r="C45" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="D45" s="16">
+      <c r="D45" s="27" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="E45" s="16">
         <v>2</v>
       </c>
-      <c r="E45" s="16"/>
       <c r="F45" s="16"/>
       <c r="G45" s="16"/>
       <c r="H45" s="16"/>
       <c r="I45" s="16"/>
       <c r="J45" s="16"/>
-      <c r="K45" s="16" t="str">
-        <f t="shared" si="0"/>
-        <v>Nu</v>
-      </c>
-      <c r="L45" s="19"/>
-    </row>
-    <row r="46" spans="1:12" ht="15.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="K45" s="16"/>
+      <c r="L45" s="16" t="str">
+        <f>IF(M45&lt;&gt;"","Da","Nu")</f>
+        <v>Nu</v>
+      </c>
+      <c r="M45" s="19"/>
+    </row>
+    <row r="46" spans="1:13" ht="15.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="8">
         <v>31</v>
       </c>
@@ -2186,22 +2441,32 @@
       <c r="C46" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="D46" s="16">
+      <c r="D46" s="27">
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
-      <c r="E46" s="16"/>
-      <c r="F46" s="16"/>
-      <c r="G46" s="16"/>
+      <c r="E46" s="16">
+        <v>2</v>
+      </c>
+      <c r="F46" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="G46" s="17" t="s">
+        <v>100</v>
+      </c>
       <c r="H46" s="16"/>
       <c r="I46" s="16"/>
       <c r="J46" s="16"/>
-      <c r="K46" s="16" t="str">
-        <f t="shared" si="0"/>
-        <v>Nu</v>
-      </c>
-      <c r="L46" s="19"/>
-    </row>
-    <row r="47" spans="1:12" ht="15.65" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="K46" s="16"/>
+      <c r="L46" s="16" t="str">
+        <f>IF(M46&lt;&gt;"","Da","Nu")</f>
+        <v>Da</v>
+      </c>
+      <c r="M46" s="19" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" ht="15.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="8">
         <v>32</v>
       </c>
@@ -2211,22 +2476,26 @@
       <c r="C47" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="D47" s="16">
+      <c r="D47" s="27" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="E47" s="16">
         <v>2</v>
       </c>
-      <c r="E47" s="16"/>
       <c r="F47" s="16"/>
       <c r="G47" s="16"/>
       <c r="H47" s="16"/>
       <c r="I47" s="16"/>
       <c r="J47" s="16"/>
-      <c r="K47" s="16" t="str">
-        <f t="shared" si="0"/>
-        <v>Nu</v>
-      </c>
-      <c r="L47" s="19"/>
-    </row>
-    <row r="48" spans="1:12" ht="15.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="K47" s="16"/>
+      <c r="L47" s="16" t="str">
+        <f>IF(M47&lt;&gt;"","Da","Nu")</f>
+        <v>Nu</v>
+      </c>
+      <c r="M47" s="19"/>
+    </row>
+    <row r="48" spans="1:13" ht="15.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="8">
         <v>33</v>
       </c>
@@ -2236,22 +2505,26 @@
       <c r="C48" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="D48" s="16">
+      <c r="D48" s="27" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="E48" s="16">
         <v>2</v>
       </c>
-      <c r="E48" s="16"/>
       <c r="F48" s="16"/>
       <c r="G48" s="16"/>
       <c r="H48" s="16"/>
       <c r="I48" s="16"/>
       <c r="J48" s="16"/>
-      <c r="K48" s="16" t="str">
-        <f t="shared" si="0"/>
-        <v>Nu</v>
-      </c>
-      <c r="L48" s="19"/>
-    </row>
-    <row r="49" spans="1:12" ht="15.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="K48" s="16"/>
+      <c r="L48" s="16" t="str">
+        <f>IF(M48&lt;&gt;"","Da","Nu")</f>
+        <v>Nu</v>
+      </c>
+      <c r="M48" s="19"/>
+    </row>
+    <row r="49" spans="1:13" ht="15.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="8">
         <v>34</v>
       </c>
@@ -2261,22 +2534,30 @@
       <c r="C49" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="D49" s="16">
+      <c r="D49" s="27">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="E49" s="16">
         <v>2</v>
       </c>
-      <c r="E49" s="16"/>
-      <c r="F49" s="16"/>
+      <c r="F49" s="17" t="s">
+        <v>100</v>
+      </c>
       <c r="G49" s="16"/>
       <c r="H49" s="16"/>
       <c r="I49" s="16"/>
       <c r="J49" s="16"/>
-      <c r="K49" s="16" t="str">
-        <f t="shared" si="0"/>
-        <v>Nu</v>
-      </c>
-      <c r="L49" s="19"/>
-    </row>
-    <row r="50" spans="1:12" ht="15.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="K49" s="16"/>
+      <c r="L49" s="16" t="str">
+        <f>IF(M49&lt;&gt;"","Da","Nu")</f>
+        <v>Da</v>
+      </c>
+      <c r="M49" s="19" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" ht="15.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="8">
         <v>35</v>
       </c>
@@ -2286,28 +2567,38 @@
       <c r="C50" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="D50" s="16">
+      <c r="D50" s="27">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="E50" s="16">
         <v>2</v>
       </c>
-      <c r="E50" s="17" t="s">
-        <v>100</v>
-      </c>
       <c r="F50" s="17" t="s">
         <v>100</v>
       </c>
-      <c r="G50" s="16"/>
-      <c r="H50" s="16"/>
-      <c r="I50" s="16"/>
-      <c r="J50" s="16"/>
-      <c r="K50" s="16" t="str">
-        <f t="shared" si="0"/>
+      <c r="G50" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="H50" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="I50" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="J50" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="K50" s="16"/>
+      <c r="L50" s="16" t="str">
+        <f>IF(M50&lt;&gt;"","Da","Nu")</f>
         <v>Da</v>
       </c>
-      <c r="L50" s="19" t="s">
+      <c r="M50" s="19" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="51" spans="1:12" ht="15.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:13" ht="15.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="8">
         <v>36</v>
       </c>
@@ -2317,22 +2608,26 @@
       <c r="C51" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="D51" s="16">
+      <c r="D51" s="27" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="E51" s="16">
         <v>2</v>
       </c>
-      <c r="E51" s="16"/>
       <c r="F51" s="16"/>
       <c r="G51" s="16"/>
       <c r="H51" s="16"/>
       <c r="I51" s="16"/>
       <c r="J51" s="16"/>
-      <c r="K51" s="16" t="str">
-        <f t="shared" si="0"/>
-        <v>Nu</v>
-      </c>
-      <c r="L51" s="19"/>
-    </row>
-    <row r="52" spans="1:12" ht="15.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="K51" s="16"/>
+      <c r="L51" s="16" t="str">
+        <f>IF(M51&lt;&gt;"","Da","Nu")</f>
+        <v>Nu</v>
+      </c>
+      <c r="M51" s="19"/>
+    </row>
+    <row r="52" spans="1:13" ht="15.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="8">
         <v>37</v>
       </c>
@@ -2342,26 +2637,34 @@
       <c r="C52" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="D52" s="16">
+      <c r="D52" s="27">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="E52" s="16">
         <v>2</v>
       </c>
-      <c r="E52" s="17" t="s">
-        <v>100</v>
-      </c>
-      <c r="F52" s="16"/>
+      <c r="F52" s="17" t="s">
+        <v>100</v>
+      </c>
       <c r="G52" s="16"/>
       <c r="H52" s="16"/>
-      <c r="I52" s="16"/>
-      <c r="J52" s="16"/>
-      <c r="K52" s="16" t="str">
-        <f t="shared" si="0"/>
+      <c r="I52" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="J52" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="K52" s="16"/>
+      <c r="L52" s="16" t="str">
+        <f>IF(M52&lt;&gt;"","Da","Nu")</f>
         <v>Da</v>
       </c>
-      <c r="L52" s="20" t="s">
+      <c r="M52" s="20" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="53" spans="1:12" ht="15.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:13" ht="15.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="8">
         <v>38</v>
       </c>
@@ -2371,22 +2674,26 @@
       <c r="C53" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="D53" s="16">
+      <c r="D53" s="27" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="E53" s="16">
         <v>2</v>
       </c>
-      <c r="E53" s="16"/>
       <c r="F53" s="16"/>
       <c r="G53" s="16"/>
       <c r="H53" s="16"/>
       <c r="I53" s="16"/>
       <c r="J53" s="16"/>
-      <c r="K53" s="16" t="str">
-        <f t="shared" si="0"/>
-        <v>Nu</v>
-      </c>
-      <c r="L53" s="19"/>
-    </row>
-    <row r="54" spans="1:12" ht="15.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="K53" s="16"/>
+      <c r="L53" s="16" t="str">
+        <f>IF(M53&lt;&gt;"","Da","Nu")</f>
+        <v>Nu</v>
+      </c>
+      <c r="M53" s="19"/>
+    </row>
+    <row r="54" spans="1:13" ht="15.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="8">
         <v>39</v>
       </c>
@@ -2396,22 +2703,26 @@
       <c r="C54" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="D54" s="16">
+      <c r="D54" s="27" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="E54" s="16">
         <v>2</v>
       </c>
-      <c r="E54" s="16"/>
       <c r="F54" s="16"/>
       <c r="G54" s="16"/>
       <c r="H54" s="16"/>
       <c r="I54" s="16"/>
       <c r="J54" s="16"/>
-      <c r="K54" s="16" t="str">
-        <f t="shared" si="0"/>
-        <v>Nu</v>
-      </c>
-      <c r="L54" s="19"/>
-    </row>
-    <row r="55" spans="1:12" ht="15.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="K54" s="16"/>
+      <c r="L54" s="16" t="str">
+        <f>IF(M54&lt;&gt;"","Da","Nu")</f>
+        <v>Nu</v>
+      </c>
+      <c r="M54" s="19"/>
+    </row>
+    <row r="55" spans="1:13" ht="15.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="8">
         <v>40</v>
       </c>
@@ -2421,22 +2732,26 @@
       <c r="C55" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="D55" s="16">
+      <c r="D55" s="27" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="E55" s="16">
         <v>2</v>
       </c>
-      <c r="E55" s="16"/>
       <c r="F55" s="16"/>
       <c r="G55" s="16"/>
       <c r="H55" s="16"/>
       <c r="I55" s="16"/>
       <c r="J55" s="16"/>
-      <c r="K55" s="16" t="str">
-        <f t="shared" si="0"/>
-        <v>Nu</v>
-      </c>
-      <c r="L55" s="19"/>
-    </row>
-    <row r="56" spans="1:12" ht="15.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="K55" s="16"/>
+      <c r="L55" s="16" t="str">
+        <f>IF(M55&lt;&gt;"","Da","Nu")</f>
+        <v>Nu</v>
+      </c>
+      <c r="M55" s="19"/>
+    </row>
+    <row r="56" spans="1:13" ht="15.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" s="8">
         <v>41</v>
       </c>
@@ -2446,12 +2761,13 @@
       <c r="C56" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="D56" s="16">
+      <c r="D56" s="27">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="E56" s="16">
         <v>2</v>
       </c>
-      <c r="E56" s="17" t="s">
-        <v>100</v>
-      </c>
       <c r="F56" s="17" t="s">
         <v>100</v>
       </c>
@@ -2464,16 +2780,19 @@
       <c r="I56" s="17" t="s">
         <v>100</v>
       </c>
-      <c r="J56" s="16"/>
-      <c r="K56" s="16" t="str">
-        <f t="shared" si="0"/>
+      <c r="J56" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="K56" s="16"/>
+      <c r="L56" s="16" t="str">
+        <f>IF(M56&lt;&gt;"","Da","Nu")</f>
         <v>Da</v>
       </c>
-      <c r="L56" s="19" t="s">
+      <c r="M56" s="19" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="57" spans="1:12" ht="15.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:13" ht="15.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" s="8">
         <v>42</v>
       </c>
@@ -2483,22 +2802,26 @@
       <c r="C57" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="D57" s="16">
+      <c r="D57" s="27" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="E57" s="16">
         <v>2</v>
       </c>
-      <c r="E57" s="16"/>
       <c r="F57" s="16"/>
       <c r="G57" s="16"/>
       <c r="H57" s="16"/>
       <c r="I57" s="16"/>
       <c r="J57" s="16"/>
-      <c r="K57" s="16" t="str">
-        <f t="shared" si="0"/>
-        <v>Nu</v>
-      </c>
-      <c r="L57" s="19"/>
-    </row>
-    <row r="58" spans="1:12" ht="15.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="K57" s="16"/>
+      <c r="L57" s="16" t="str">
+        <f>IF(M57&lt;&gt;"","Da","Nu")</f>
+        <v>Nu</v>
+      </c>
+      <c r="M57" s="19"/>
+    </row>
+    <row r="58" spans="1:13" ht="15.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" s="8">
         <v>43</v>
       </c>
@@ -2508,26 +2831,36 @@
       <c r="C58" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="D58" s="16">
+      <c r="D58" s="27">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="E58" s="16">
         <v>2</v>
       </c>
-      <c r="E58" s="17" t="s">
-        <v>100</v>
-      </c>
-      <c r="F58" s="16"/>
+      <c r="F58" s="17" t="s">
+        <v>100</v>
+      </c>
       <c r="G58" s="16"/>
-      <c r="H58" s="16"/>
-      <c r="I58" s="16"/>
-      <c r="J58" s="16"/>
-      <c r="K58" s="16" t="str">
-        <f t="shared" si="0"/>
+      <c r="H58" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="I58" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="J58" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="K58" s="16"/>
+      <c r="L58" s="16" t="str">
+        <f>IF(M58&lt;&gt;"","Da","Nu")</f>
         <v>Da</v>
       </c>
-      <c r="L58" s="19" t="s">
+      <c r="M58" s="19" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="59" spans="1:12" ht="15.65" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:13" ht="15.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" s="8">
         <v>44</v>
       </c>
@@ -2537,26 +2870,30 @@
       <c r="C59" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="D59" s="16">
+      <c r="D59" s="27">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="E59" s="16">
         <v>2</v>
       </c>
-      <c r="E59" s="17" t="s">
-        <v>100</v>
-      </c>
-      <c r="F59" s="16"/>
+      <c r="F59" s="17" t="s">
+        <v>100</v>
+      </c>
       <c r="G59" s="16"/>
       <c r="H59" s="16"/>
       <c r="I59" s="16"/>
       <c r="J59" s="16"/>
-      <c r="K59" s="16" t="str">
-        <f t="shared" si="0"/>
+      <c r="K59" s="16"/>
+      <c r="L59" s="16" t="str">
+        <f>IF(M59&lt;&gt;"","Da","Nu")</f>
         <v>Da</v>
       </c>
-      <c r="L59" s="19" t="s">
+      <c r="M59" s="19" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="60" spans="1:12" ht="15.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:13" ht="15.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" s="8">
         <v>45</v>
       </c>
@@ -2566,449 +2903,542 @@
       <c r="C60" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="D60" s="16">
+      <c r="D60" s="27" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="E60" s="16">
         <v>2</v>
       </c>
-      <c r="E60" s="16"/>
       <c r="F60" s="16"/>
       <c r="G60" s="16"/>
       <c r="H60" s="16"/>
       <c r="I60" s="16"/>
       <c r="J60" s="16"/>
-      <c r="K60" s="16" t="str">
-        <f t="shared" si="0"/>
-        <v>Nu</v>
-      </c>
-      <c r="L60" s="19"/>
-    </row>
-    <row r="61" spans="1:12" ht="15.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="K60" s="16"/>
+      <c r="L60" s="16" t="str">
+        <f>IF(M60&lt;&gt;"","Da","Nu")</f>
+        <v>Nu</v>
+      </c>
+      <c r="M60" s="19"/>
+    </row>
+    <row r="61" spans="1:13" ht="15.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61" s="8">
-        <v>46</v>
-      </c>
-      <c r="B61" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="C61" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="D61" s="16">
+        <v>49</v>
+      </c>
+      <c r="B61" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E61" s="16"/>
-      <c r="F61" s="16"/>
-      <c r="G61" s="16"/>
-      <c r="H61" s="16"/>
-      <c r="I61" s="16"/>
-      <c r="J61" s="16"/>
-      <c r="K61" s="16" t="str">
-        <f t="shared" si="0"/>
-        <v>Nu</v>
-      </c>
-      <c r="L61" s="19"/>
-    </row>
-    <row r="62" spans="1:12" ht="15.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C61" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="D61" s="27">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="E61" s="16">
+        <v>3</v>
+      </c>
+      <c r="F61" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="G61" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="H61" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="I61" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="J61" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="K61" s="16"/>
+      <c r="L61" s="16" t="str">
+        <f>IF(M61&lt;&gt;"","Da","Nu")</f>
+        <v>Da</v>
+      </c>
+      <c r="M61" s="20" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13" ht="15.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" s="8">
-        <v>47</v>
-      </c>
-      <c r="B62" s="9" t="s">
-        <v>88</v>
-      </c>
-      <c r="C62" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="D62" s="16">
-        <v>2</v>
-      </c>
-      <c r="E62" s="17" t="s">
-        <v>100</v>
-      </c>
-      <c r="F62" s="17" t="s">
-        <v>100</v>
-      </c>
-      <c r="G62" s="17" t="s">
-        <v>100</v>
-      </c>
-      <c r="H62" s="17" t="s">
-        <v>100</v>
-      </c>
+        <v>50</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C62" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="D62" s="27" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="E62" s="16">
+        <v>3</v>
+      </c>
+      <c r="F62" s="16"/>
+      <c r="G62" s="16"/>
+      <c r="H62" s="16"/>
       <c r="I62" s="16"/>
       <c r="J62" s="16"/>
-      <c r="K62" s="16" t="str">
-        <f t="shared" si="0"/>
-        <v>Da</v>
-      </c>
-      <c r="L62" s="20" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="63" spans="1:12" ht="15.65" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="K62" s="16"/>
+      <c r="L62" s="16" t="str">
+        <f>IF(M62&lt;&gt;"","Da","Nu")</f>
+        <v>Nu</v>
+      </c>
+      <c r="M62" s="19"/>
+    </row>
+    <row r="63" spans="1:13" ht="15.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" s="8">
-        <v>48</v>
-      </c>
-      <c r="B63" s="9" t="s">
-        <v>89</v>
-      </c>
-      <c r="C63" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="D63" s="16">
-        <v>2</v>
-      </c>
-      <c r="E63" s="17" t="s">
-        <v>100</v>
+        <v>51</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C63" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D63" s="27">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="E63" s="16">
+        <v>3</v>
       </c>
       <c r="F63" s="17" t="s">
         <v>100</v>
       </c>
-      <c r="G63" s="17" t="s">
-        <v>100</v>
-      </c>
+      <c r="G63" s="16"/>
       <c r="H63" s="16"/>
       <c r="I63" s="16"/>
       <c r="J63" s="16"/>
-      <c r="K63" s="16" t="str">
-        <f t="shared" si="0"/>
-        <v>Da</v>
-      </c>
-      <c r="L63" s="19" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="64" spans="1:12" ht="15.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="K63" s="16"/>
+      <c r="L63" s="16" t="str">
+        <f>IF(M63&lt;&gt;"","Da","Nu")</f>
+        <v>Nu</v>
+      </c>
+      <c r="M63" s="19"/>
+    </row>
+    <row r="64" spans="1:13" ht="15.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A64" s="8">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C64" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="D64" s="16">
-        <v>3</v>
-      </c>
-      <c r="E64" s="17" t="s">
-        <v>100</v>
-      </c>
-      <c r="F64" s="17" t="s">
-        <v>100</v>
-      </c>
-      <c r="G64" s="17" t="s">
-        <v>100</v>
-      </c>
-      <c r="H64" s="17" t="s">
-        <v>100</v>
-      </c>
-      <c r="I64" s="17" t="s">
-        <v>100</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="D64" s="27" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="E64" s="16">
+        <v>3</v>
+      </c>
+      <c r="F64" s="16"/>
+      <c r="G64" s="16"/>
+      <c r="H64" s="16"/>
+      <c r="I64" s="16"/>
       <c r="J64" s="16"/>
-      <c r="K64" s="16" t="str">
-        <f t="shared" si="0"/>
-        <v>Da</v>
-      </c>
-      <c r="L64" s="20" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="65" spans="1:12" ht="15.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="K64" s="16"/>
+      <c r="L64" s="16" t="str">
+        <f>IF(M64&lt;&gt;"","Da","Nu")</f>
+        <v>Nu</v>
+      </c>
+      <c r="M64" s="19"/>
+    </row>
+    <row r="65" spans="1:13" ht="15.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A65" s="8">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C65" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="D65" s="16">
-        <v>3</v>
-      </c>
-      <c r="E65" s="16"/>
-      <c r="F65" s="16"/>
-      <c r="G65" s="16"/>
-      <c r="H65" s="16"/>
+      <c r="D65" s="27">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="E65" s="16">
+        <v>3</v>
+      </c>
+      <c r="F65" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="G65" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="H65" s="17" t="s">
+        <v>100</v>
+      </c>
       <c r="I65" s="16"/>
       <c r="J65" s="16"/>
-      <c r="K65" s="16" t="str">
-        <f t="shared" si="0"/>
-        <v>Nu</v>
-      </c>
-      <c r="L65" s="19"/>
-    </row>
-    <row r="66" spans="1:12" ht="15.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="K65" s="16"/>
+      <c r="L65" s="16" t="str">
+        <f>IF(M65&lt;&gt;"","Da","Nu")</f>
+        <v>Da</v>
+      </c>
+      <c r="M65" s="19" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="66" spans="1:13" ht="15.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A66" s="8">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C66" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="D66" s="16">
-        <v>3</v>
-      </c>
-      <c r="E66" s="16"/>
-      <c r="F66" s="16"/>
-      <c r="G66" s="16"/>
-      <c r="H66" s="16"/>
+      <c r="D66" s="27">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="E66" s="16">
+        <v>3</v>
+      </c>
+      <c r="F66" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="G66" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="H66" s="17" t="s">
+        <v>100</v>
+      </c>
       <c r="I66" s="16"/>
       <c r="J66" s="16"/>
-      <c r="K66" s="16" t="str">
-        <f t="shared" si="0"/>
-        <v>Nu</v>
-      </c>
-      <c r="L66" s="19"/>
-    </row>
-    <row r="67" spans="1:12" ht="15.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="K66" s="16"/>
+      <c r="L66" s="16" t="str">
+        <f>IF(M66&lt;&gt;"","Da","Nu")</f>
+        <v>Da</v>
+      </c>
+      <c r="M66" s="19" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="67" spans="1:13" ht="15.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A67" s="8">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C67" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="D67" s="16">
-        <v>3</v>
-      </c>
-      <c r="E67" s="16"/>
-      <c r="F67" s="16"/>
-      <c r="G67" s="16"/>
-      <c r="H67" s="16"/>
+        <v>3</v>
+      </c>
+      <c r="D67" s="27">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="E67" s="16">
+        <v>3</v>
+      </c>
+      <c r="F67" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="G67" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="H67" s="17" t="s">
+        <v>100</v>
+      </c>
       <c r="I67" s="16"/>
       <c r="J67" s="16"/>
-      <c r="K67" s="16" t="str">
-        <f t="shared" si="0"/>
-        <v>Nu</v>
-      </c>
-      <c r="L67" s="19"/>
-    </row>
-    <row r="68" spans="1:12" ht="15.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="K67" s="16"/>
+      <c r="L67" s="16" t="str">
+        <f>IF(M67&lt;&gt;"","Da","Nu")</f>
+        <v>Da</v>
+      </c>
+      <c r="M67" s="19" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="68" spans="1:13" ht="15.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68" s="8">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C68" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="D68" s="16">
-        <v>3</v>
-      </c>
-      <c r="E68" s="16"/>
+        <v>6</v>
+      </c>
+      <c r="D68" s="27" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="E68" s="16">
+        <v>3</v>
+      </c>
       <c r="F68" s="16"/>
       <c r="G68" s="16"/>
       <c r="H68" s="16"/>
       <c r="I68" s="16"/>
       <c r="J68" s="16"/>
-      <c r="K68" s="16" t="str">
-        <f t="shared" si="0"/>
-        <v>Nu</v>
-      </c>
-      <c r="L68" s="19"/>
-    </row>
-    <row r="69" spans="1:12" ht="15.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="K68" s="16"/>
+      <c r="L68" s="16" t="str">
+        <f>IF(M68&lt;&gt;"","Da","Nu")</f>
+        <v>Nu</v>
+      </c>
+      <c r="M68" s="19"/>
+    </row>
+    <row r="69" spans="1:13" ht="15.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A69" s="8">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C69" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="D69" s="27">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="E69" s="16">
+        <v>3</v>
+      </c>
+      <c r="F69" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="G69" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="H69" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="I69" s="16"/>
+      <c r="J69" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="K69" s="16"/>
+      <c r="L69" s="16" t="str">
+        <f>IF(M69&lt;&gt;"","Da","Nu")</f>
+        <v>Da</v>
+      </c>
+      <c r="M69" s="19" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="70" spans="1:13" ht="15.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A70" s="8">
+        <v>58</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C70" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="D69" s="16">
-        <v>3</v>
-      </c>
-      <c r="E69" s="16"/>
-      <c r="F69" s="16"/>
-      <c r="G69" s="16"/>
-      <c r="H69" s="16"/>
-      <c r="I69" s="16"/>
-      <c r="J69" s="16"/>
-      <c r="K69" s="16" t="str">
-        <f t="shared" si="0"/>
-        <v>Nu</v>
-      </c>
-      <c r="L69" s="19"/>
-    </row>
-    <row r="70" spans="1:12" ht="15.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A70" s="8">
-        <v>55</v>
-      </c>
-      <c r="B70" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C70" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="D70" s="16">
-        <v>3</v>
-      </c>
-      <c r="E70" s="16"/>
+      <c r="D70" s="27" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="E70" s="16">
+        <v>3</v>
+      </c>
       <c r="F70" s="16"/>
       <c r="G70" s="16"/>
       <c r="H70" s="16"/>
       <c r="I70" s="16"/>
       <c r="J70" s="16"/>
-      <c r="K70" s="16" t="str">
-        <f t="shared" si="0"/>
-        <v>Nu</v>
-      </c>
-      <c r="L70" s="19"/>
-    </row>
-    <row r="71" spans="1:12" ht="15.65" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="K70" s="16"/>
+      <c r="L70" s="16" t="str">
+        <f>IF(M70&lt;&gt;"","Da","Nu")</f>
+        <v>Nu</v>
+      </c>
+      <c r="M70" s="19"/>
+    </row>
+    <row r="71" spans="1:13" ht="15.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A71" s="8">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C71" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="D71" s="16">
-        <v>3</v>
-      </c>
-      <c r="E71" s="16"/>
+        <v>3</v>
+      </c>
+      <c r="D71" s="27" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="E71" s="16">
+        <v>3</v>
+      </c>
       <c r="F71" s="16"/>
       <c r="G71" s="16"/>
       <c r="H71" s="16"/>
       <c r="I71" s="16"/>
       <c r="J71" s="16"/>
-      <c r="K71" s="16" t="str">
-        <f t="shared" si="0"/>
-        <v>Nu</v>
-      </c>
-      <c r="L71" s="19"/>
-    </row>
-    <row r="72" spans="1:12" ht="15.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="K71" s="16"/>
+      <c r="L71" s="16" t="str">
+        <f>IF(M71&lt;&gt;"","Da","Nu")</f>
+        <v>Nu</v>
+      </c>
+      <c r="M71" s="19"/>
+    </row>
+    <row r="72" spans="1:13" ht="15.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A72" s="8">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C72" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="D72" s="16">
-        <v>3</v>
-      </c>
-      <c r="E72" s="17" t="s">
-        <v>100</v>
-      </c>
-      <c r="F72" s="17" t="s">
-        <v>100</v>
-      </c>
-      <c r="G72" s="17" t="s">
-        <v>100</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="D72" s="27" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="E72" s="16">
+        <v>3</v>
+      </c>
+      <c r="F72" s="16"/>
+      <c r="G72" s="16"/>
       <c r="H72" s="16"/>
       <c r="I72" s="16"/>
       <c r="J72" s="16"/>
-      <c r="K72" s="16" t="str">
-        <f t="shared" si="0"/>
-        <v>Da</v>
-      </c>
-      <c r="L72" s="19" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="73" spans="1:12" ht="15.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="K72" s="16"/>
+      <c r="L72" s="16" t="str">
+        <f>IF(M72&lt;&gt;"","Da","Nu")</f>
+        <v>Nu</v>
+      </c>
+      <c r="M72" s="19"/>
+    </row>
+    <row r="73" spans="1:13" ht="15.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A73" s="8">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C73" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="D73" s="16">
-        <v>3</v>
-      </c>
-      <c r="E73" s="16"/>
-      <c r="F73" s="16"/>
-      <c r="G73" s="16"/>
-      <c r="H73" s="16"/>
+      <c r="D73" s="27">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="E73" s="16">
+        <v>3</v>
+      </c>
+      <c r="F73" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="G73" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="H73" s="17" t="s">
+        <v>100</v>
+      </c>
       <c r="I73" s="16"/>
-      <c r="J73" s="16"/>
-      <c r="K73" s="16" t="str">
-        <f t="shared" si="0"/>
-        <v>Nu</v>
-      </c>
-      <c r="L73" s="19"/>
-    </row>
-    <row r="74" spans="1:12" ht="15.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J73" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="K73" s="16"/>
+      <c r="L73" s="16" t="str">
+        <f>IF(M73&lt;&gt;"","Da","Nu")</f>
+        <v>Da</v>
+      </c>
+      <c r="M73" s="19" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="74" spans="1:13" ht="15.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A74" s="8">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C74" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="D74" s="16">
-        <v>3</v>
-      </c>
-      <c r="E74" s="16"/>
+      <c r="D74" s="27" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="E74" s="16">
+        <v>3</v>
+      </c>
       <c r="F74" s="16"/>
       <c r="G74" s="16"/>
       <c r="H74" s="16"/>
       <c r="I74" s="16"/>
       <c r="J74" s="16"/>
-      <c r="K74" s="16" t="str">
-        <f t="shared" si="0"/>
-        <v>Nu</v>
-      </c>
-      <c r="L74" s="19"/>
-    </row>
-    <row r="75" spans="1:12" ht="15.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="K74" s="16"/>
+      <c r="L74" s="16" t="str">
+        <f>IF(M74&lt;&gt;"","Da","Nu")</f>
+        <v>Nu</v>
+      </c>
+      <c r="M74" s="19"/>
+    </row>
+    <row r="75" spans="1:13" ht="15.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A75" s="8">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C75" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="D75" s="16">
-        <v>3</v>
-      </c>
-      <c r="E75" s="16"/>
-      <c r="F75" s="16"/>
-      <c r="G75" s="16"/>
+      <c r="D75" s="27">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="E75" s="16">
+        <v>3</v>
+      </c>
+      <c r="F75" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="G75" s="17" t="s">
+        <v>100</v>
+      </c>
       <c r="H75" s="16"/>
-      <c r="I75" s="16"/>
-      <c r="J75" s="16"/>
-      <c r="K75" s="16" t="str">
-        <f t="shared" si="0"/>
-        <v>Nu</v>
-      </c>
-      <c r="L75" s="19"/>
-    </row>
-    <row r="76" spans="1:12" ht="15.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I75" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="J75" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="K75" s="16"/>
+      <c r="L75" s="16" t="str">
+        <f>IF(M75&lt;&gt;"","Da","Nu")</f>
+        <v>Nu</v>
+      </c>
+      <c r="M75" s="19"/>
+    </row>
+    <row r="76" spans="1:13" ht="15.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A76" s="8">
-        <v>61</v>
-      </c>
-      <c r="B76" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C76" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="D76" s="16">
-        <v>3</v>
-      </c>
-      <c r="E76" s="17" t="s">
-        <v>100</v>
+        <v>46</v>
+      </c>
+      <c r="B76" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="C76" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="D76" s="27">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="E76" s="16">
+        <v>2</v>
       </c>
       <c r="F76" s="17" t="s">
         <v>100</v>
@@ -3016,82 +3446,106 @@
       <c r="G76" s="17" t="s">
         <v>100</v>
       </c>
-      <c r="H76" s="16"/>
-      <c r="I76" s="16"/>
-      <c r="J76" s="16"/>
-      <c r="K76" s="16" t="str">
-        <f t="shared" si="0"/>
+      <c r="H76" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="I76" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="J76" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="K76" s="16"/>
+      <c r="L76" s="16" t="str">
+        <f>IF(M76&lt;&gt;"","Da","Nu")</f>
         <v>Da</v>
       </c>
-      <c r="L76" s="19" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="77" spans="1:12" ht="15.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M76" s="19" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="77" spans="1:13" ht="15.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A77" s="8">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C77" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="D77" s="16">
-        <v>3</v>
-      </c>
-      <c r="E77" s="16"/>
-      <c r="F77" s="16"/>
-      <c r="G77" s="16"/>
-      <c r="H77" s="16"/>
+      <c r="D77" s="27">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="E77" s="16">
+        <v>3</v>
+      </c>
+      <c r="F77" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="G77" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="H77" s="17" t="s">
+        <v>100</v>
+      </c>
       <c r="I77" s="16"/>
       <c r="J77" s="16"/>
-      <c r="K77" s="16" t="str">
-        <f t="shared" si="0"/>
-        <v>Nu</v>
-      </c>
-      <c r="L77" s="19"/>
-    </row>
-    <row r="78" spans="1:12" ht="15.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="K77" s="16"/>
+      <c r="L77" s="16" t="str">
+        <f>IF(M77&lt;&gt;"","Da","Nu")</f>
+        <v>Da</v>
+      </c>
+      <c r="M77" s="19" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="78" spans="1:13" ht="15.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A78" s="8">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C78" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="D78" s="16">
-        <v>3</v>
-      </c>
-      <c r="E78" s="16"/>
+      <c r="D78" s="27" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="E78" s="16">
+        <v>3</v>
+      </c>
       <c r="F78" s="16"/>
       <c r="G78" s="16"/>
       <c r="H78" s="16"/>
       <c r="I78" s="16"/>
       <c r="J78" s="16"/>
-      <c r="K78" s="16" t="str">
-        <f t="shared" si="0"/>
-        <v>Nu</v>
-      </c>
-      <c r="L78" s="19"/>
-    </row>
-    <row r="79" spans="1:12" ht="15.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="K78" s="16"/>
+      <c r="L78" s="16" t="str">
+        <f>IF(M78&lt;&gt;"","Da","Nu")</f>
+        <v>Nu</v>
+      </c>
+      <c r="M78" s="19"/>
+    </row>
+    <row r="79" spans="1:13" ht="15.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A79" s="8">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C79" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="D79" s="16">
-        <v>3</v>
-      </c>
-      <c r="E79" s="17" t="s">
-        <v>100</v>
+        <v>6</v>
+      </c>
+      <c r="D79" s="27">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="E79" s="16">
+        <v>3</v>
       </c>
       <c r="F79" s="17" t="s">
         <v>100</v>
@@ -3099,262 +3553,376 @@
       <c r="G79" s="17" t="s">
         <v>100</v>
       </c>
-      <c r="H79" s="16"/>
-      <c r="I79" s="16"/>
-      <c r="J79" s="16"/>
-      <c r="K79" s="16" t="str">
-        <f t="shared" si="0"/>
+      <c r="H79" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="I79" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="J79" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="K79" s="16"/>
+      <c r="L79" s="16" t="str">
+        <f>IF(M79&lt;&gt;"","Da","Nu")</f>
         <v>Da</v>
       </c>
-      <c r="L79" s="19" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="80" spans="1:12" ht="15.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M79" s="19" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="80" spans="1:13" ht="15.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A80" s="8">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C80" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="D80" s="16">
-        <v>3</v>
-      </c>
-      <c r="E80" s="16"/>
+      <c r="D80" s="27" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="E80" s="16">
+        <v>3</v>
+      </c>
       <c r="F80" s="16"/>
       <c r="G80" s="16"/>
       <c r="H80" s="16"/>
       <c r="I80" s="16"/>
       <c r="J80" s="16"/>
-      <c r="K80" s="16" t="str">
-        <f t="shared" si="0"/>
-        <v>Nu</v>
-      </c>
-      <c r="L80" s="19"/>
-    </row>
-    <row r="81" spans="1:12" ht="15.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="K80" s="16"/>
+      <c r="L80" s="16" t="str">
+        <f>IF(M80&lt;&gt;"","Da","Nu")</f>
+        <v>Nu</v>
+      </c>
+      <c r="M80" s="19"/>
+    </row>
+    <row r="81" spans="1:13" ht="15.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A81" s="8">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C81" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="D81" s="16">
-        <v>3</v>
-      </c>
-      <c r="E81" s="16"/>
+        <v>3</v>
+      </c>
+      <c r="D81" s="27" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="E81" s="16">
+        <v>3</v>
+      </c>
       <c r="F81" s="16"/>
       <c r="G81" s="16"/>
       <c r="H81" s="16"/>
       <c r="I81" s="16"/>
       <c r="J81" s="16"/>
-      <c r="K81" s="16" t="str">
-        <f t="shared" ref="K81:K88" si="1">IF(L81&lt;&gt;"","Da","Nu")</f>
-        <v>Nu</v>
-      </c>
-      <c r="L81" s="19"/>
-    </row>
-    <row r="82" spans="1:12" ht="15.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="K81" s="16"/>
+      <c r="L81" s="16" t="str">
+        <f>IF(M81&lt;&gt;"","Da","Nu")</f>
+        <v>Nu</v>
+      </c>
+      <c r="M81" s="19"/>
+    </row>
+    <row r="82" spans="1:13" ht="15.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A82" s="8">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C82" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="D82" s="16">
-        <v>3</v>
-      </c>
-      <c r="E82" s="16"/>
-      <c r="F82" s="16"/>
-      <c r="G82" s="16"/>
-      <c r="H82" s="16"/>
+        <v>3</v>
+      </c>
+      <c r="D82" s="27">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="E82" s="16">
+        <v>3</v>
+      </c>
+      <c r="F82" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="G82" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="H82" s="17" t="s">
+        <v>100</v>
+      </c>
       <c r="I82" s="16"/>
       <c r="J82" s="16"/>
-      <c r="K82" s="16" t="str">
-        <f t="shared" si="1"/>
-        <v>Nu</v>
-      </c>
-      <c r="L82" s="19"/>
-    </row>
-    <row r="83" spans="1:12" ht="15.65" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="K82" s="16"/>
+      <c r="L82" s="16" t="str">
+        <f>IF(M82&lt;&gt;"","Da","Nu")</f>
+        <v>Da</v>
+      </c>
+      <c r="M82" s="19" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="83" spans="1:13" ht="15.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A83" s="8">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C83" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="D83" s="16">
-        <v>3</v>
-      </c>
-      <c r="E83" s="16"/>
+        <v>6</v>
+      </c>
+      <c r="D83" s="27" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="E83" s="16">
+        <v>3</v>
+      </c>
       <c r="F83" s="16"/>
       <c r="G83" s="16"/>
       <c r="H83" s="16"/>
       <c r="I83" s="16"/>
       <c r="J83" s="16"/>
-      <c r="K83" s="16" t="str">
-        <f t="shared" si="1"/>
-        <v>Nu</v>
-      </c>
-      <c r="L83" s="19"/>
-    </row>
-    <row r="84" spans="1:12" ht="15.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="K83" s="16"/>
+      <c r="L83" s="16" t="str">
+        <f>IF(M83&lt;&gt;"","Da","Nu")</f>
+        <v>Nu</v>
+      </c>
+      <c r="M83" s="19"/>
+    </row>
+    <row r="84" spans="1:13" ht="15.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A84" s="8">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C84" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="D84" s="16">
-        <v>3</v>
-      </c>
-      <c r="E84" s="16"/>
-      <c r="F84" s="16"/>
-      <c r="G84" s="16"/>
-      <c r="H84" s="16"/>
-      <c r="I84" s="16"/>
-      <c r="J84" s="16"/>
-      <c r="K84" s="16" t="str">
-        <f t="shared" si="1"/>
-        <v>Nu</v>
-      </c>
-      <c r="L84" s="19"/>
-    </row>
-    <row r="85" spans="1:12" ht="15.25" customHeight="1" x14ac:dyDescent="0.3">
+        <v>6</v>
+      </c>
+      <c r="D84" s="27">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="E84" s="16">
+        <v>3</v>
+      </c>
+      <c r="F84" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="G84" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="H84" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="I84" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="J84" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="K84" s="16"/>
+      <c r="L84" s="16" t="str">
+        <f>IF(M84&lt;&gt;"","Da","Nu")</f>
+        <v>Da</v>
+      </c>
+      <c r="M84" s="19" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="85" spans="1:13" ht="15.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A85" s="8">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C85" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="D85" s="16">
-        <v>3</v>
-      </c>
-      <c r="E85" s="16"/>
-      <c r="F85" s="16"/>
+      <c r="D85" s="27">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="E85" s="16">
+        <v>3</v>
+      </c>
+      <c r="F85" s="17" t="s">
+        <v>100</v>
+      </c>
       <c r="G85" s="16"/>
       <c r="H85" s="16"/>
       <c r="I85" s="16"/>
       <c r="J85" s="16"/>
-      <c r="K85" s="16" t="str">
-        <f t="shared" si="1"/>
-        <v>Nu</v>
-      </c>
-      <c r="L85" s="19"/>
-    </row>
-    <row r="86" spans="1:12" ht="15.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="K85" s="16"/>
+      <c r="L85" s="16" t="str">
+        <f>IF(M85&lt;&gt;"","Da","Nu")</f>
+        <v>Nu</v>
+      </c>
+      <c r="M85" s="19"/>
+    </row>
+    <row r="86" spans="1:13" ht="15.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A86" s="8">
-        <v>71</v>
-      </c>
-      <c r="B86" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C86" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="D86" s="16">
-        <v>3</v>
+        <v>73</v>
+      </c>
+      <c r="B86" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="C86" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="D86" s="27">
+        <f t="shared" si="2"/>
+        <v>2</v>
       </c>
       <c r="E86" s="17" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="F86" s="17" t="s">
         <v>100</v>
       </c>
-      <c r="G86" s="16"/>
+      <c r="G86" s="17" t="s">
+        <v>100</v>
+      </c>
       <c r="H86" s="16"/>
       <c r="I86" s="16"/>
       <c r="J86" s="16"/>
-      <c r="K86" s="16" t="str">
-        <f t="shared" si="1"/>
+      <c r="K86" s="16"/>
+      <c r="L86" s="16" t="str">
+        <f>IF(M86&lt;&gt;"","Da","Nu")</f>
+        <v>Nu</v>
+      </c>
+      <c r="M86" s="19"/>
+    </row>
+    <row r="87" spans="1:13" ht="15.65" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A87" s="8">
+        <v>47</v>
+      </c>
+      <c r="B87" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="C87" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="D87" s="27">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="E87" s="16">
+        <v>2</v>
+      </c>
+      <c r="F87" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="G87" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="H87" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="I87" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="J87" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="K87" s="16"/>
+      <c r="L87" s="16" t="str">
+        <f>IF(M87&lt;&gt;"","Da","Nu")</f>
         <v>Da</v>
       </c>
-      <c r="L86" s="19" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="87" spans="1:12" ht="15.65" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A87" s="8">
-        <v>72</v>
-      </c>
-      <c r="B87" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C87" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="D87" s="16">
-        <v>3</v>
-      </c>
-      <c r="E87" s="16"/>
-      <c r="F87" s="16"/>
-      <c r="G87" s="16"/>
-      <c r="H87" s="16"/>
-      <c r="I87" s="16"/>
-      <c r="J87" s="16"/>
-      <c r="K87" s="16" t="str">
-        <f t="shared" si="1"/>
-        <v>Nu</v>
-      </c>
-      <c r="L87" s="19"/>
-    </row>
-    <row r="88" spans="1:12" ht="15.65" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A88" s="8">
-        <v>73</v>
-      </c>
-      <c r="B88" s="9" t="s">
-        <v>114</v>
-      </c>
-      <c r="C88" s="12" t="s">
+      <c r="M87" s="20" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="88" spans="1:13" ht="15.65" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A88" s="22">
+        <v>74</v>
+      </c>
+      <c r="B88" s="24" t="s">
+        <v>127</v>
+      </c>
+      <c r="C88" s="26"/>
+      <c r="D88" s="27">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="E88" s="17" t="s">
         <v>105</v>
       </c>
-      <c r="D88" s="17" t="s">
-        <v>105</v>
-      </c>
-      <c r="E88" s="17" t="s">
-        <v>100</v>
-      </c>
-      <c r="F88" s="17" t="s">
-        <v>100</v>
-      </c>
-      <c r="G88" s="16"/>
-      <c r="H88" s="16"/>
-      <c r="I88" s="16"/>
-      <c r="J88" s="16"/>
-      <c r="K88" s="16" t="str">
-        <f t="shared" si="1"/>
-        <v>Nu</v>
-      </c>
+      <c r="F88" s="20" t="s">
+        <v>100</v>
+      </c>
+      <c r="G88" s="19"/>
+      <c r="H88" s="19"/>
+      <c r="I88" s="19"/>
+      <c r="J88" s="19"/>
+      <c r="K88" s="19"/>
       <c r="L88" s="19"/>
-    </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B90" s="3" t="s">
+      <c r="M88" s="19" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="89" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A89" s="23">
+        <v>48</v>
+      </c>
+      <c r="B89" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="C89" s="27" t="s">
+        <v>43</v>
+      </c>
+      <c r="D89" s="27">
+        <f t="shared" ref="D89" si="3">IF(COUNTA(F89:K89)=0,"",COUNTA(F89:K89))</f>
+        <v>4</v>
+      </c>
+      <c r="E89" s="4">
+        <v>2</v>
+      </c>
+      <c r="F89" s="21" t="s">
+        <v>100</v>
+      </c>
+      <c r="G89" s="21" t="s">
+        <v>100</v>
+      </c>
+      <c r="H89" s="21" t="s">
+        <v>100</v>
+      </c>
+      <c r="I89" s="21" t="s">
+        <v>100</v>
+      </c>
+      <c r="J89" s="4"/>
+      <c r="K89" s="4"/>
+      <c r="L89" s="4" t="str">
+        <f>IF(M89&lt;&gt;"","Da","Nu")</f>
+        <v>Da</v>
+      </c>
+      <c r="M89" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="93" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B93" s="3" t="s">
         <v>119</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A15:M15" xr:uid="{35A61541-D905-407A-8E1F-46C41C720BC2}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A16:M89">
+      <sortCondition ref="B15"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <webPublishItems count="1">
-    <webPublishItem id="19688" divId="LC-lab-info1s1_19688" sourceType="range" sourceRef="A1:J88" destinationFile="https://storage.rcs-rds.ro/dav/Digi%20Cloud/Ovidius_Studenti/INFO1s1/Копия%20LC-lab-info1s1.htm" title="Lista studentilor care au incarcat lab pe server"/>
+    <webPublishItem id="19688" divId="LC-lab-info1s1_19688" sourceType="range" sourceRef="A1:K88" destinationFile="https://storage.rcs-rds.ro/dav/Digi%20Cloud/Ovidius_Studenti/INFO1s1/Копия%20LC-lab-info1s1.htm" title="Lista studentilor care au incarcat lab pe server"/>
   </webPublishItems>
 </worksheet>
 </file>
</xml_diff>